<commit_message>
Adding reader for BigDecimal
</commit_message>
<xml_diff>
--- a/src/test/resources/files/with_all_java_types.xlsx
+++ b/src/test/resources/files/with_all_java_types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Desktop\example\src\test\resources\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFB1038-B066-4D4C-B3BC-A4DA6E9296CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{579309BD-D44F-4B4C-8417-CDE6E25407A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>str_value</t>
   </si>
@@ -92,13 +92,22 @@
   </si>
   <si>
     <t>54.4</t>
+  </si>
+  <si>
+    <t>big_decimal_value</t>
+  </si>
+  <si>
+    <t>3294832483943920</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000000"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -108,6 +117,14 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="204"/>
@@ -134,7 +151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -143,6 +160,10 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="12" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -361,10 +382,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -374,9 +395,10 @@
     <col min="5" max="5" width="19.1328125" customWidth="1"/>
     <col min="6" max="6" width="23.3984375" customWidth="1"/>
     <col min="7" max="7" width="20.3984375" customWidth="1"/>
+    <col min="12" max="12" width="46.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -410,8 +432,11 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="8" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -441,8 +466,11 @@
       <c r="K2" s="1">
         <v>1</v>
       </c>
+      <c r="L2" s="11">
+        <v>-323344343.22349</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -470,8 +498,11 @@
         <v>6573</v>
       </c>
       <c r="K3" s="5"/>
+      <c r="L3" s="10" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
@@ -500,6 +531,9 @@
       </c>
       <c r="K4" s="1">
         <v>127</v>
+      </c>
+      <c r="L4" s="9">
+        <v>93249932943949</v>
       </c>
     </row>
   </sheetData>

</xml_diff>